<commit_message>
generic commit message, Wed 13:59:41 09.08.2023.
</commit_message>
<xml_diff>
--- a/babb03 cropping table.xlsx
+++ b/babb03 cropping table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\imageProcessTif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EC2F41-4FE1-4908-A647-1849A3187C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6C2FD9-0602-4946-9D1F-651606F07AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{2D0EAEAB-47F1-498F-A59D-91F173EB47DA}"/>
+    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{2D0EAEAB-47F1-498F-A59D-91F173EB47DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -678,7 +678,7 @@
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1142,8 +1142,7 @@
         <v>33</v>
       </c>
       <c r="N6" s="6">
-        <f>ROUND((K6+(4677/2)),0)</f>
-        <v>5143</v>
+        <v>5056</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>32</v>
@@ -1247,13 +1246,11 @@
       <c r="V7" s="4">
         <v>500</v>
       </c>
-      <c r="W7" s="1">
-        <f t="shared" si="6"/>
-        <v>13</v>
-      </c>
-      <c r="X7" s="6">
-        <f t="shared" si="7"/>
-        <v>511</v>
+      <c r="W7" s="7">
+        <v>2</v>
+      </c>
+      <c r="X7" s="7">
+        <v>500</v>
       </c>
       <c r="Y7" s="2">
         <f t="shared" si="8"/>

</xml_diff>